<commit_message>
add 1 test result
</commit_message>
<xml_diff>
--- a/马萧萧高中成绩/成绩趋势.xlsx
+++ b/马萧萧高中成绩/成绩趋势.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\james_home\local_src\codebase\马萧萧高中成绩\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4D0329-3620-4F43-B229-D111F1E7187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAB2A84-D482-48EA-BD35-341B36C6C042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>化学</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>总分</t>
+  </si>
+  <si>
+    <t>三上G12模拟</t>
   </si>
 </sst>
 </file>
@@ -290,11 +293,68 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -315,6 +375,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -345,6 +408,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,11 +460,68 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -419,6 +542,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -449,6 +575,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,11 +627,68 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -523,6 +709,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -553,6 +742,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>127.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -602,11 +794,68 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -627,6 +876,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -657,6 +909,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -706,11 +961,68 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -731,6 +1043,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -761,6 +1076,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,11 +1128,68 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -835,6 +1210,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -865,6 +1243,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1254,7 +1635,7 @@
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -1275,6 +1656,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1305,6 +1689,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>582.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>578</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,7 +1802,7 @@
             <c:strRef>
               <c:f>平时成绩!$B$1:$O$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>二上10月份</c:v>
                 </c:pt>
@@ -1436,6 +1823,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>二下期末</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>三上G12模拟</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1466,6 +1856,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3140,10 +3533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W46" sqref="W46"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -3153,9 +3546,10 @@
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3177,8 +3571,11 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3203,8 +3600,11 @@
       <c r="H2">
         <v>103</v>
       </c>
+      <c r="I2">
+        <v>104</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3229,8 +3629,11 @@
       <c r="H3">
         <v>83</v>
       </c>
+      <c r="I3">
+        <v>90</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3255,8 +3658,11 @@
       <c r="H4">
         <v>127.5</v>
       </c>
+      <c r="I4">
+        <v>124</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3281,8 +3687,11 @@
       <c r="H5">
         <v>90</v>
       </c>
+      <c r="I5">
+        <v>81</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -3307,8 +3716,11 @@
       <c r="H6">
         <v>81</v>
       </c>
+      <c r="I6">
+        <v>94</v>
+      </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3333,8 +3745,11 @@
       <c r="H7">
         <v>98</v>
       </c>
+      <c r="I7">
+        <v>85</v>
+      </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -3366,8 +3781,11 @@
         <f>SUM(H2:H7)</f>
         <v>582.5</v>
       </c>
+      <c r="I8">
+        <v>578</v>
+      </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3391,6 +3809,9 @@
       </c>
       <c r="H9">
         <v>476</v>
+      </c>
+      <c r="I9">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3402,4 +3823,10 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{4327cfd9-47ed-48f1-9376-4ab3148935bb}" enabled="1" method="Privileged" siteId="{5d471751-9675-428d-917b-70f44f9630b0}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>